<commit_message>
Check difference in backgrounds that use same sprite
</commit_message>
<xml_diff>
--- a/Doco/BackgroundToSprites.xlsx
+++ b/Doco/BackgroundToSprites.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\ExileMappedBackground\Doco\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C548B906-8A68-4DBF-9D1B-1063C14DEECE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="25875" windowHeight="11310"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="130">
   <si>
     <t>4e</t>
   </si>
@@ -379,12 +385,39 @@
   </si>
   <si>
     <t>red cyan yellow is one…</t>
+  </si>
+  <si>
+    <t>water</t>
+  </si>
+  <si>
+    <t>hollow wall</t>
+  </si>
+  <si>
+    <t>solid wall</t>
+  </si>
+  <si>
+    <t>background_object_from_type</t>
+  </si>
+  <si>
+    <t>one usage where player lies down at beginning when grenading door</t>
+  </si>
+  <si>
+    <t>green so looks like shrubery - not solid</t>
+  </si>
+  <si>
+    <t>standard solid partial wall</t>
+  </si>
+  <si>
+    <t>handle_background_object_emerging (yellow / white)</t>
+  </si>
+  <si>
+    <t>red/magenta (within ship)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -435,6 +468,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -482,7 +518,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -515,9 +551,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -550,6 +603,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -725,22 +795,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="1"/>
-    <col min="5" max="5" width="29.140625" customWidth="1"/>
-    <col min="6" max="33" width="9.140625" style="4"/>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.1640625" style="1"/>
+    <col min="5" max="5" width="29.1640625" customWidth="1"/>
+    <col min="6" max="33" width="9.1640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>95</v>
       </c>
@@ -754,7 +824,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>55</v>
       </c>
@@ -801,7 +871,7 @@
       <c r="AF2" s="4"/>
       <c r="AG2" s="4"/>
     </row>
-    <row r="3" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>74</v>
       </c>
@@ -848,7 +918,7 @@
       <c r="AF3" s="4"/>
       <c r="AG3" s="4"/>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>45</v>
       </c>
@@ -862,7 +932,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -876,7 +946,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -890,7 +960,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -937,7 +1007,7 @@
       <c r="AF7" s="4"/>
       <c r="AG7" s="4"/>
     </row>
-    <row r="8" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>30</v>
       </c>
@@ -984,7 +1054,7 @@
       <c r="AF8" s="4"/>
       <c r="AG8" s="4"/>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
         <v>89</v>
       </c>
@@ -998,7 +1068,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -1012,7 +1082,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
         <v>61</v>
       </c>
@@ -1026,7 +1096,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
         <v>62</v>
       </c>
@@ -1040,7 +1110,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
         <v>80</v>
       </c>
@@ -1054,7 +1124,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
         <v>81</v>
       </c>
@@ -1068,7 +1138,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
         <v>83</v>
       </c>
@@ -1082,7 +1152,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
@@ -1096,7 +1166,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
         <v>87</v>
       </c>
@@ -1110,7 +1180,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
         <v>47</v>
       </c>
@@ -1124,7 +1194,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
         <v>77</v>
       </c>
@@ -1138,7 +1208,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
         <v>78</v>
       </c>
@@ -1152,7 +1222,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
         <v>92</v>
       </c>
@@ -1166,7 +1236,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
         <v>86</v>
       </c>
@@ -1180,7 +1250,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A23" s="1" t="s">
         <v>91</v>
       </c>
@@ -1194,7 +1264,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A24" s="1" t="s">
         <v>76</v>
       </c>
@@ -1208,7 +1278,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A25" s="1" t="s">
         <v>69</v>
       </c>
@@ -1222,7 +1292,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
         <v>32</v>
       </c>
@@ -1236,7 +1306,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
         <v>88</v>
       </c>
@@ -1250,7 +1320,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A28" s="1" t="s">
         <v>31</v>
       </c>
@@ -1264,7 +1334,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
         <v>11</v>
       </c>
@@ -1280,7 +1350,9 @@
       <c r="E29" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="F29" s="4"/>
+      <c r="F29" s="2" t="s">
+        <v>121</v>
+      </c>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
@@ -1309,7 +1381,7 @@
       <c r="AF29" s="4"/>
       <c r="AG29" s="4"/>
     </row>
-    <row r="30" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A30" s="2" t="s">
         <v>56</v>
       </c>
@@ -1325,7 +1397,9 @@
       <c r="E30" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="F30" s="4"/>
+      <c r="F30" s="2" t="s">
+        <v>122</v>
+      </c>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
@@ -1354,7 +1428,7 @@
       <c r="AF30" s="4"/>
       <c r="AG30" s="4"/>
     </row>
-    <row r="31" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A31" s="2" t="s">
         <v>22</v>
       </c>
@@ -1370,7 +1444,9 @@
       <c r="E31" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="F31" s="4"/>
+      <c r="F31" s="2" t="s">
+        <v>123</v>
+      </c>
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
@@ -1399,7 +1475,7 @@
       <c r="AF31" s="4"/>
       <c r="AG31" s="4"/>
     </row>
-    <row r="32" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A32" s="1" t="s">
         <v>1</v>
       </c>
@@ -1413,7 +1489,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A33" s="2" t="s">
         <v>43</v>
       </c>
@@ -1429,7 +1505,9 @@
       <c r="E33" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="F33" s="4"/>
+      <c r="F33" s="2" t="s">
+        <v>124</v>
+      </c>
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
@@ -1458,7 +1536,7 @@
       <c r="AF33" s="4"/>
       <c r="AG33" s="4"/>
     </row>
-    <row r="34" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A34" s="2" t="s">
         <v>23</v>
       </c>
@@ -1474,7 +1552,9 @@
       <c r="E34" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="F34" s="4"/>
+      <c r="F34" s="2" t="s">
+        <v>125</v>
+      </c>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
@@ -1503,7 +1583,7 @@
       <c r="AF34" s="4"/>
       <c r="AG34" s="4"/>
     </row>
-    <row r="35" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A35" s="1" t="s">
         <v>71</v>
       </c>
@@ -1517,7 +1597,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A36" s="1" t="s">
         <v>3</v>
       </c>
@@ -1531,7 +1611,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A37" s="1" t="s">
         <v>90</v>
       </c>
@@ -1545,7 +1625,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="38" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A38" s="1" t="s">
         <v>21</v>
       </c>
@@ -1559,7 +1639,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A39" s="2" t="s">
         <v>53</v>
       </c>
@@ -1575,7 +1655,9 @@
       <c r="E39" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="F39" s="4"/>
+      <c r="F39" s="2" t="s">
+        <v>126</v>
+      </c>
       <c r="G39" s="4"/>
       <c r="H39" s="4"/>
       <c r="I39" s="4"/>
@@ -1604,7 +1686,7 @@
       <c r="AF39" s="4"/>
       <c r="AG39" s="4"/>
     </row>
-    <row r="40" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A40" s="2" t="s">
         <v>29</v>
       </c>
@@ -1620,7 +1702,9 @@
       <c r="E40" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="F40" s="4"/>
+      <c r="F40" s="2" t="s">
+        <v>127</v>
+      </c>
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
@@ -1649,7 +1733,7 @@
       <c r="AF40" s="4"/>
       <c r="AG40" s="4"/>
     </row>
-    <row r="41" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A41" s="1" t="s">
         <v>51</v>
       </c>
@@ -1663,7 +1747,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A42" s="1" t="s">
         <v>25</v>
       </c>
@@ -1677,7 +1761,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="43" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A43" s="1" t="s">
         <v>50</v>
       </c>
@@ -1691,7 +1775,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A44" s="1" t="s">
         <v>57</v>
       </c>
@@ -1705,7 +1789,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="45" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A45" s="1" t="s">
         <v>34</v>
       </c>
@@ -1719,7 +1803,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="46" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A46" s="1" t="s">
         <v>37</v>
       </c>
@@ -1733,7 +1817,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="47" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A47" s="1" t="s">
         <v>40</v>
       </c>
@@ -1747,7 +1831,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="48" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A48" s="1" t="s">
         <v>41</v>
       </c>
@@ -1761,7 +1845,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="49" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A49" s="1" t="s">
         <v>42</v>
       </c>
@@ -1775,7 +1859,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="50" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A50" s="1" t="s">
         <v>44</v>
       </c>
@@ -1789,7 +1873,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="51" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A51" s="1" t="s">
         <v>9</v>
       </c>
@@ -1803,7 +1887,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="52" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A52" s="1" t="s">
         <v>12</v>
       </c>
@@ -1817,7 +1901,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="53" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A53" s="1" t="s">
         <v>68</v>
       </c>
@@ -1831,7 +1915,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="54" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A54" s="1" t="s">
         <v>59</v>
       </c>
@@ -1845,7 +1929,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="55" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A55" s="1" t="s">
         <v>63</v>
       </c>
@@ -1859,7 +1943,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="56" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A56" s="1" t="s">
         <v>66</v>
       </c>
@@ -1873,7 +1957,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="57" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A57" s="1" t="s">
         <v>27</v>
       </c>
@@ -1887,7 +1971,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="58" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A58" s="1" t="s">
         <v>39</v>
       </c>
@@ -1901,7 +1985,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="59" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A59" s="1" t="s">
         <v>72</v>
       </c>
@@ -1915,7 +1999,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="60" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A60" s="1" t="s">
         <v>46</v>
       </c>
@@ -1929,7 +2013,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="61" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A61" s="1" t="s">
         <v>33</v>
       </c>
@@ -1943,7 +2027,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="62" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A62" s="1" t="s">
         <v>13</v>
       </c>
@@ -1957,7 +2041,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="63" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A63" s="2" t="s">
         <v>6</v>
       </c>
@@ -1973,7 +2057,9 @@
       <c r="E63" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="F63" s="4"/>
+      <c r="F63" s="4" t="s">
+        <v>128</v>
+      </c>
       <c r="G63" s="4"/>
       <c r="H63" s="4"/>
       <c r="I63" s="4"/>
@@ -2002,7 +2088,7 @@
       <c r="AF63" s="4"/>
       <c r="AG63" s="4"/>
     </row>
-    <row r="64" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A64" s="2" t="s">
         <v>24</v>
       </c>
@@ -2018,7 +2104,9 @@
       <c r="E64" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="F64" s="4"/>
+      <c r="F64" s="2" t="s">
+        <v>129</v>
+      </c>
       <c r="G64" s="4"/>
       <c r="H64" s="4"/>
       <c r="I64" s="4"/>
@@ -2047,7 +2135,7 @@
       <c r="AF64" s="4"/>
       <c r="AG64" s="4"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A65" s="1" t="s">
         <v>48</v>
       </c>
@@ -2071,24 +2159,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>